<commit_message>
Puntos con R mas facil.
</commit_message>
<xml_diff>
--- a/Puntos.xlsx
+++ b/Puntos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f472c84d2004e08b/Documentos/Laboratorio5robotica/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f472c84d2004e08b/Documentos/Lab5Robotica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{286832A7-DC00-4F8E-9465-2D11778036AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{286832A7-DC00-4F8E-9465-2D11778036AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15816016-0AC0-499C-A11E-27112A1D5924}"/>
   <bookViews>
-    <workbookView xWindow="5664" yWindow="1572" windowWidth="17280" windowHeight="8964" xr2:uid="{E17E7B05-96A9-46CD-8E53-0B2D87B165F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E17E7B05-96A9-46CD-8E53-0B2D87B165F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>Base Marcador</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Centro</t>
-  </si>
-  <si>
-    <t>Rad</t>
   </si>
   <si>
     <t>M</t>
@@ -96,12 +93,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,20 +436,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC882874-8921-4B2B-9A48-2C4498D2BE81}">
-  <dimension ref="A2:E62"/>
+  <dimension ref="A2:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -453,7 +457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>-14.3704</v>
       </c>
@@ -461,12 +465,12 @@
         <v>-211.14359999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -474,7 +478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>48.003599999999999</v>
       </c>
@@ -482,7 +486,7 @@
         <v>-264.41770000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>23.107399999999998</v>
       </c>
@@ -490,7 +494,7 @@
         <v>-195.59559999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>50.7226</v>
       </c>
@@ -498,32 +502,23 @@
         <v>-185.60589999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11">
-        <v>55.512</v>
+        <v>63.779499999999999</v>
       </c>
       <c r="C11">
-        <v>-201.48560000000001</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11">
-        <v>16.586200000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-187.10679999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12">
-        <v>34.351599999999998</v>
+        <v>71.254800000000003</v>
       </c>
       <c r="C12">
-        <v>-226.67850000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-206.70699999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>59.465000000000003</v>
       </c>
@@ -531,362 +526,378 @@
         <v>-217.59379999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14">
+        <v>34.351599999999998</v>
+      </c>
+      <c r="C14">
+        <v>-226.67850000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>59.465000000000003</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-217.59379999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16">
         <v>90.283500000000004</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>-247.35489999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>101.898</v>
-      </c>
-      <c r="C18">
-        <v>-242.6651</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>77.723699999999994</v>
-      </c>
-      <c r="C19">
-        <v>-175.8383</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>101.5656</v>
+        <v>101.898</v>
       </c>
       <c r="C20">
-        <v>-191.095</v>
+        <v>-242.6651</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21">
-        <v>109.78740000000001</v>
+        <v>77.723699999999994</v>
       </c>
       <c r="C21">
-        <v>-164.23939999999999</v>
+        <v>-175.8383</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22">
+        <v>101.5656</v>
+      </c>
+      <c r="C22">
+        <v>-191.095</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>109.78740000000001</v>
+      </c>
+      <c r="C23">
+        <v>-164.23939999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24">
         <v>133.54759999999999</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <v>-229.89490000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>208.78550000000001</v>
-      </c>
-      <c r="C26">
-        <v>-164.54740000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27">
-        <v>156.74260000000001</v>
-      </c>
-      <c r="C27">
-        <v>-91.1203</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28">
-        <v>246.3537</v>
+        <v>208.78550000000001</v>
       </c>
       <c r="C28">
-        <v>-82.763400000000004</v>
+        <v>-164.54740000000001</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29">
+        <v>156.74260000000001</v>
+      </c>
+      <c r="C29">
+        <v>-91.1203</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>246.3537</v>
+      </c>
+      <c r="C30">
+        <v>-82.763400000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31">
         <v>208.78550000000001</v>
       </c>
-      <c r="C29">
+      <c r="C31">
         <v>-164.54740000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>229.26830000000001</v>
+      </c>
+      <c r="C35">
+        <v>-0.89939999999999998</v>
+      </c>
+      <c r="D35" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+      <c r="E35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
         <v>1</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C38" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33">
-        <v>229.26830000000001</v>
-      </c>
-      <c r="C33">
-        <v>-0.89939999999999998</v>
-      </c>
-      <c r="D33" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B39">
         <v>171.2176</v>
       </c>
-      <c r="C37">
+      <c r="C39">
         <v>72.344800000000006</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B38">
-        <v>254.953</v>
-      </c>
-      <c r="C38">
-        <v>91.253500000000003</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>2</v>
-      </c>
-      <c r="B39">
-        <v>251.01769999999999</v>
-      </c>
-      <c r="C39">
-        <v>108.6808</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40">
+        <v>254.953</v>
+      </c>
+      <c r="C40">
+        <v>91.253500000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>251.01769999999999</v>
+      </c>
+      <c r="C41">
+        <v>108.6808</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
         <v>167.28219999999999</v>
       </c>
-      <c r="C40">
+      <c r="C42">
         <v>89.772199999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>163.34690000000001</v>
+      </c>
+      <c r="C43">
+        <v>107.1995</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44">
+        <v>247.0823</v>
+      </c>
+      <c r="C44">
+        <v>126.1082</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
         <v>3</v>
       </c>
-      <c r="B41">
-        <v>163.34690000000001</v>
-      </c>
-      <c r="C41">
-        <v>107.1995</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B42">
-        <v>247.0823</v>
-      </c>
-      <c r="C42">
-        <v>126.1082</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
         <v>1</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B46">
-        <v>142.18369999999999</v>
-      </c>
-      <c r="C46">
-        <v>128.47290000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B47">
-        <v>131.30019999999999</v>
-      </c>
-      <c r="C47">
-        <v>166.96379999999999</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B48">
-        <v>170.11199999999999</v>
+        <v>142.18369999999999</v>
       </c>
       <c r="C48">
-        <v>157.2869</v>
+        <v>128.47290000000001</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B49">
-        <v>159.0865</v>
+        <v>131.30019999999999</v>
       </c>
       <c r="C49">
-        <v>195.73740000000001</v>
+        <v>166.96379999999999</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B50">
+        <v>170.11199999999999</v>
+      </c>
+      <c r="C50">
+        <v>157.2869</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>159.0865</v>
+      </c>
+      <c r="C51">
+        <v>195.73740000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B52">
         <v>197.81540000000001</v>
       </c>
-      <c r="C50">
+      <c r="C52">
         <v>186.0812</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
         <v>1</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C55" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54">
-        <v>68.347099999999998</v>
-      </c>
-      <c r="C54">
-        <v>227.10589999999999</v>
-      </c>
-      <c r="D54" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55">
-        <v>58.460700000000003</v>
-      </c>
-      <c r="C55">
-        <v>183.4425</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B56">
-        <v>36.976900000000001</v>
+        <v>68.347099999999998</v>
       </c>
       <c r="C56">
-        <v>258.3655</v>
+        <v>227.10589999999999</v>
+      </c>
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56">
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B57">
-        <v>112.6039</v>
+        <v>58.460700000000003</v>
       </c>
       <c r="C57">
-        <v>239.5095</v>
+        <v>183.4425</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B58">
-        <v>58.460700000000003</v>
+        <v>36.976900000000001</v>
       </c>
       <c r="C58">
-        <v>183.4425</v>
+        <v>258.3655</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B59">
-        <v>64.508700000000005</v>
+        <v>112.6039</v>
       </c>
       <c r="C59">
-        <v>207.69990000000001</v>
+        <v>239.5095</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
       <c r="B60">
-        <v>55.555500000000002</v>
+        <v>58.460700000000003</v>
       </c>
       <c r="C60">
-        <v>241.63720000000001</v>
+        <v>183.4425</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B61">
-        <v>88.572400000000002</v>
+        <v>64.508700000000005</v>
       </c>
       <c r="C61">
-        <v>232.61859999999999</v>
+        <v>207.69990000000001</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B62">
+        <v>55.555500000000002</v>
+      </c>
+      <c r="C62">
+        <v>241.63720000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>88.572400000000002</v>
+      </c>
+      <c r="C63">
+        <v>232.61859999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64">
         <v>64.508700000000005</v>
       </c>
-      <c r="C62">
+      <c r="C64">
         <v>207.69990000000001</v>
       </c>
     </row>

</xml_diff>